<commit_message>
Draft app complete now jigger with prompts
</commit_message>
<xml_diff>
--- a/TimeEntryData.xlsx
+++ b/TimeEntryData.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V4"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -524,21 +524,6 @@
           <t>Narrative</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>Body</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>Subject</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>Alias</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -599,185 +584,7 @@
       <c r="R2" t="inlineStr"/>
       <c r="S2" t="inlineStr">
         <is>
-          <t>Email communication with Imran Rahman concerning case assessment and scheduling interviews with Ramiro Gonzalez's former supervisors.</t>
-        </is>
-      </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>Of course. 
-Nicole Tavis
-One Embarcadero Center | Suite 2100 | San Francisco | CA | 94111
-PH 415-578-6900 | DIR 415.604.0209 
-From: Daniel Cravens &lt;dcravens@ohaganmeyer.com&gt; 
-Sent: Thursday, July 25, 2024 12:52 PM
-To: Nicole Tavis &lt;ntavis@ohaganmeyer.com&gt;
-Cc: Imran Rahman &lt;irahman@ohaganmeyer.com&gt;
-Subject: FW: Ramiro Gonzalez v. DS Electric, Inc. - Berkley Claim No.: 49538 [EXTERNAL] [IMAN-ACTIVE.FID448525]
-Hi Nicole,
-Would you please plug this into letter head to Daniel and Heather.  
-Thank you!
-Daniel J. Cravens
-Fresno Managing Partner
-8050 N. Palm Ave. | Suite 300 | Fresno | CA | 93711
-DIR 415.604.0142 | CEL 559.472.6584
-From: Imran Rahman &lt;irahman@ohaganmeyer.com &lt;mailto:irahman@ohaganmeyer.com&gt; &gt; 
-Sent: Monday, July 15, 2024 4:54 PM
-To: Daniel Cravens &lt;dcravens@ohaganmeyer.com &lt;mailto:dcravens@ohaganmeyer.com&gt; &gt;
-Subject: FW: Ramiro Gonzalez v. DS Electric, Inc. - Berkley Claim No.: 49538 [EXTERNAL] [IMAN-ACTIVE.FID448525]
-Here is the updated assessment. I highlighted things the supervisor told me. 
-“Good morning, everyone, 
-We are writing to provide you with the assessment below in light of the ongoing settlement discussions between the parties. Ramino Gonzalez’s  (“Gonzalez”) December 13, 2023 demand letter puts forth Labor Code Claims based on retaliation, failure to provide uninterrupted meal and rest breaks, failure to pay overtime, reimburse for necessary expenditures, provide accurate wage statements, and waiting time penalties. In short, Gonzalez claims he was retaliated against and wrongfully terminated after he questioned whether DSE was paying him appropriately. DSE’s position is that he was laid off due to lack of work. 
-To date we have interviewed the President of DSE, Daniel Suarez (“Suarez”), Foreman Jorge Tovar (“Tovar”), reviewed Gonazlez’s earning statements, timecards, and mandatory weekly filings made by DSE to the California Department of Industrial Relations (“DIR”) regarding how much DSE was paying Gonzalez for the hours he worked. 
-Factual Summary
-1.	Gonzalez Was Hired As  Residential Electrician, Given A Company Vehicle And Debit Card.
-Between September 11, 2021 – September 8, 2023, Gonzalez was employed by DSE as non-exempt hourly “Residential Electrician” (“Inside-Wireman”). His job duties included electrical work performed for residential construction.  Up until the last three months of his employment, Gonzalez worked in the Fresno area in a position that had a “prevailing wage” set by the DIR.  As such, on a weekly basis, DSE must submit to the DIR the number of regulated employees it employs, the hours they have worked, and how much they were paid. The final maximum mandatory wage rate applicable for Gonzalez’s position at the time was $26.93 per hour. Gonzalez’s final rate of pay at DSE was $27 per hour. (Exhibit 1)
-Although Gonzalez claims he was not paid for overtime, we substantiated that he received overtime pay when he worked overtime hours. Gonzalez’s time records from DSE show that he consistently received overtime pay up until April 8, 2022.  (Id. at DSE 000051-117) Thereafter, Gonzalez worked overtime infrequently, working some overtime in June 2022, but ceased doing so for the remainder of his employment. (Id. at DSE 000014-50)
-We have not seen any DSE policies on meal and rest breaks. Based on the timecards provided by DSE, Gonzalez entered his own time with his own handwriting on printed timecards.  The timecards provided by DSE show Gonzalez’s worked Monday through Friday, starting at either 6:00 or 7:00 a.m., and ending at 2:30 or 3:30 p.m. (Exhibit 2) There is no indication of a 30-minute unpaid meal break or of rest breaks taken. However, generally, next to each day there is a handwritten “8,” or weekly total “40” handwritten. Given there is 8 hours and 30 minutes of time worked on each of these days, this signifies Gonzalez’s thirty-minute unpaid lunch break. Based on our interview of Tovar, Gonzalez’s former supervisor, DSE provided at least two fifteen-minute rest breaks, at around 9:00 a.m. and before 1:30 p.m., and at least a thirty-minute lunch break at around 11:00 a.m.
-Prior to June 2023, Gonzalez worked on a single project where DSE was hired by a subcontractor, Valley Unique Electric, working on a project for the General Contractor, BJ Perch Construction.  This project was in Hanford, which is 96 miles from Atwater, where Gonzalez lived during his employment. Given the lengthy commute, while Gonzalez worked on this project, DSE gave Gonzalez a company vehicle and a debit card that was intended for gas and incidental expenditures. 
-Gonzalez claims that he was forced to purchase tools to perform work for DSE including “multiple drills, a skill saw, a level, a framing gun, batteries, a safety hat, and various other tools.”  Yet, he was given a debit card for precisely these types of purchases. Nevertheless, Gonzalez alleges that he asked DSE to compensate him for these expenditures, but it failed to do so. We have been unable to substantiate these allegations.
-2.	Gonzalez Was Questioned About Why He Was Asking About His Pay Relative To Others. 
-In June 2023, Tovar was notified by BJ Perch that Gonzalez was asking other trades at the job site, specifically plumbers, how much they made and complaining that he did not make as much as them. Tovar then notified Suarez that Gonzalez was asking other trades at the project what they were earning relative to Gonzalez’s pay. Saurez immediately contacted Gonzalez. When Suarez spoke to Gonazlez on the phone, he says told Gonzalez, “Stop talking to everybody and getting me and trouble,” and asked him, “Why don’t you ask me about what’s going on?” Gonzalez replied that he was “I’m just making sure you are paying what I am supposed to make.” Gonzalez was upset and claiming that DSE was underpaying him. Saurez responded that Gonzalez was not doing anything wrong but was “making the GC [general contractor] believe [DSE] is underpaying” Gonzalez. Mr. Saurez then told Gonzalez that he would send him a copy of materials from the DIR proving that DSE was paying what it was required to pay Gonzalez per the DIR. Suarez described this conversation as “not a friendly call.” 
-Suarez and Tovar then provided paperwork from the DIR specifying the prevailing wage for trades employed to their employees at the BJ Perch job site, including Gonzalez. Gonzalez’s only response to Tovar at being provided this information was that Gonzalez said he was going to review it. 
-3.	Gonzalez Was Transferred And Later Terminated Due To Lack Of Work. 
-Due to a lack of work for a residential electrician on the BJ Perch Construction Project, by June 30, 2023, DSE transferred Gonzalez to a location that was in Merced, which is less than 10 miles from Gonzalez’s residence. Given the shorter commute, both DSE and Gonzalez benefited from the shorter commute, and Gonzalez would no longer need a company card and debit card to cover fuel for the long distance drive. 
-Unfortunately, due to a continuing lack of work, on September 8, 2023, Gonzalez was laid off along with four other employees for lack of work. However, DSE does not have documentation of these terminations. We substantiated that DSE continued to have “Hiring” signage up following Gonzalez’s termination and his position has been replaced by another employee. 
-Legal Analysis
-1.	Labor Code 1102.5 Claims
-Labor Code § 1102.5 is a whistleblower statute, the purpose of which is to encourage workplace whistleblowers to report unlawful acts internally or externally without fearing retaliation. (Soukup v. Law Offices of Herbert Hafif (2006) 39 Cal.4th 260, 287.) To prevail on this claim, the plaintiff must show (1) the plaintiff engaged in protected activity, (2) the defendant subjected the plaintiff to an adverse employment action, and (3) there is a causal link between the two.  (Ross v. County of Riverside (2019) 36 Cal.App.5th 25, 36-37.) 
-“Protected activity” is defined to internal or external communications from the plaintiff that show that they in good faith communicated to their employer or a governmental investigative body that the action or conduct of the employer violates a state or federal regulation. (Green v. Ralee Engineering Co. (1998) 19 Cal.4th 66, 76-77; Mize-Kurzman v. Marin Community College Dist. (2012) 202 Cal.App.4th 832, 854.) “[O]nce the employee has made that necessary threshold showing, the employer bears ‘the burden of proof to demonstrate by clear and convincing evidence’ that the alleged adverse employment action would have occurred ‘for legitimate, independent reasons’ even if the employee had not engaged in protected whistleblowing activities.” (Lawson v. PPG Architectural Finishes, Inc. (2022) 12 Cal.5th 703, 712.) Then the plaintiff must show this explanation is merely a pretext for the retaliation.” (Manavian v. Department of Justice (2018) 28 Cal.App.5th 1127, 1141.)
-In this case, Gonzalez argues that he engaged or perceived as having engaged in protected activity when, in June 2023, he inquired with individuals at his work site, including the general contractor, about how much they were paid relative to his pay. Even if Gonzalez’s communications did not allege DSE’s violation of a law, he was at least perceived as having done so because DSE perceived he was “talking” would get the company in “trouble.” 
-Next, Gonzalez can establish that by June 30, 2022, DSE had taken away privileges of employment from him, including the company vehicle and credit card.  However, this cannot be considered an adverse employment action since it was premised upon his commute being substantially shortened.  Gonzalez will have difficulty establishing that DSE took his company vehicle and credit card away because of his communications. DSE can easily posit that Gonzalez’s new substantially shortened commute was the reason why it took its vehicle and card back from Gonzalez.
-Where Gonzalez can make stronger gains is his termination, which occurred within three months of his alleged protected activity. DSE can point to the lack of overtime as evidence that there was a lack of work and point to four other employees were terminated with Gonzalez. However,  he can rebut this argument by pointing to the hiring signs and replacement as evidence of pretext. Given the tenor of the discussion between Gonzalez and DSE about his asking what others were paid relative of him, testimony from DSE on this topic may also provide direct evidence of retaliatory animus. 
-Based on the foregoing, we assess that Gonzalez has a 45% of prevailing on his Labor Code 1102.5 claim. 
-2.	Failure to Provide Meal Periods 
-Under California Labor Code sections 226.7 and 512 and the applicable Wage Orders, an employer may not employ an employee for more than five hours per day without providing an uninterrupted meal period of not less than 30 minutes.  Employers need only “provide” and not “ensure” meal periods.  (Brinker v. Super. Ct. (2012) 53 Cal.4th 1004, 1014.)  The California Supreme Court defined this standard as “an employer must relieve the employee of all duty for the designated period, but need not ensure that the employee does not work.”  (Ibid.)  The Brinker decision also held that an employer must provide employees with meal periods at or before the completion of the fifth hour of the employees’ shifts.  (Id. at 1041.)  Thus, a meal period taken after the fifth hour of a shift can be a violation if the employee was not provided with the opportunity to take a meal period earlier.  Conversely, a violation does not occur when an employee voluntarily decides to take a late meal period or performs any work during the meal period. The statute of limitations on missed meal period claims is three years. 
-In this case, based upon the time records provided to us by DSE, there is indication that Gonzalez got a thirty-minute meal break, but whether that occurred within the fifth hour of each shift he worked is not shown in the time records. In our experience, it is not uncommon for a small percentage of meal or rest periods to be missed, late (after the 5th hour of work), or short (less than 30 minutes).  Thus, much of this claim will depend on the weight of testimony.  For example, the timing of Gonzalez’s meal periods may have been based on a personal preference.  As with his other claims, we expect Gonzalez to exaggerate and claim that he missed his meal periods every single day, which is not supported by his own timecards. Therefore, it is likely that Plaintiff will be able to establish some cognizable claim for penalties based on non-compliant meal or rest periods. 
-At this early stage, prior to Plaintiff’s deposition, we estimate a 40% chance of prevailing on Plaintiff missed meal period claims.   
-3.	Failure to Provide Rest Periods
-The California Wage Orders provide that employers shall permit employees to take one ten-minute paid rest break for every four hours of work or major fraction thereof.  However, the employer need not provide employees with a rest break when they work a shift of less than three and a half hours.    
-The Brinker decision discussed above determined that the “major fraction thereof” language, combined with the fact that employees who work fewer than three and a half hours are not entitled to a rest period, entitles employees to “10 minutes rest for shifts from three and one-half to six hours in length, 20 minutes for shifts of more than six hours up to 10 hours, 30 minutes for shifts of more than 10 hours up to 14 hours, and so on.”  Pursuant to the Wage Orders, under normal circumstances, California employers should provide an employee a ten-minute rest period in the morning, then a lunch break, and then a second rest break in the afternoon.  Normally, the rest break should be provided during the middle of the work period.    
-Under the Wage Orders, an employer merely needs to “authorize and permit” a non-exempt employee to take ten-minute paid rest periods.  An employer is not subject to any sort of penalty if an employee, who was truly authorized and permitted to take a rest break, “freely chooses without any coercion or encouragement to forego or waive a rest period.”  (DLSE Opinion Letter 2002.01.08)  The rest period premium is limited to one per day, regardless of how many rest periods an employee was entitled to.  
-DSE did not have employees capture when they took their rest periods. Again, we expect Gonzalez will exaggerate the level of non-compliance and claim that he missed his rest periods every single day. At this early stage, prior to Plaintiff’s deposition, we estimate a 50% chance of prevailing on Plaintiff missed rest period claims.   
-4.	Failure to Pay Overtime
-California Labor Code section 510 requires overtime compensation for ‘[a]ny work inexcess of eight hours in one workday and any work in excess of 40 hours in anyone workweek.’ ” (Flowers v. Los Angeles County Metropolitan Transportation Authority (2015) 243 Cal.App.4th 66, 83.)
-In this case, based upon the pay records provided to us by DSE, there is clear indication Gonzalez received overtime pay when he worked overtime hours. At this time, we are not aware of any facts that would give rise to liability for this cause of action.   
-5.	Failure to Provide Accurate Wage Statements 
-Labor Code section 226(a) requires every employer to furnish each of its employees with an itemized written statement semimonthly or at the time of each wage payment.  The statement can be a detachable part of the check, draft, or voucher paying the employee’s wage or may be furnished separately.  It must be accurate and show the following: (1) gross wages earned; (2) total hours worked by each employee; (3) the number of piece-rate units earned and any applicable piece rate if the employee is paid on a piece-rate basis; (4) all deductions; (5) net wages earned; (6) the inclusive dates of the period for which the employee is being paid; (7) the employee’s name and identification number of the last four digits of the employee’s social security number; (8) the name and address of the legal entity that is the employer; and (9) all applicable hourly rates in effect during the pay period and the corresponding number of hours worked at each hourly rate by the employee. 
-The penalty prescribed for failing to comply with these requirements is set in finite amounts, unlike meal and rest period violations, which are dependent on the employee’s hourly wage.
-Specifically, an employee can recover $50 for the initial pay period in which the employer failed to meet these requirements and $100 for every subsequent violation.  Each employee is capped at a $4,000 aggregate recovery for wage statement violations.  (Lab. Code, § 226 subd. (e).)  Failing to provide a wage statement will also result in a penalty under Section 226 subd. (e).  
-Gonzalez argues that the wage statements are not compliant based on Defendant’s failure to pay minimum wages and missed meal and/or rest period premium payments.  Fortunately, there is no legal support for these claims.  In fact, a recent California Court of Appeals case established that employees cannot recover derivative penalties under Labor Code section 226. (Naranjo, et al. v. Spectrum Security Services, Inc., (2019) 40 Cal. App. 5th 444, (citing Maldonado v. Epsilon Plastics, Inc. (2018) 22 Cal. App. 5th 1308.) 
-At this time, we are not aware of any facts that would give rise to liability for this cause of action.   
-6.	Waiting Time Penalties 
-Generally, an employer who discharges an employee must immediately pay the employee all wages earned.  (Lab. Code § 201.)  The California Supreme Court has made it clear that this obligation arises whether an employee is involuntarily terminated from an ongoing employment relationship, as when an employer fires an employee, or when an employer releases an employee after completion of the specific job assignment or time duration for which the employee was hired.  (Smith v. Superior Court (2006) 39 Cal.4th 77, 81.)  
-An employer that willfully fails to pay any wages to a former employee without abatement or reduction within the specified time frame for an employee who is discharged or resigns may be assessed waiting time penalties in accordance with Labor Code section 203.  If the penalties are assessed, the employer will owe an amount in addition to the unpaid wages equal to the employee’s daily wages for each day the wages remain unpaid, capped at thirty days’ wages.  The penalty is not limited by the number of workdays an employee might have worked during the month.  Rather, once the daily rate is calculated, it is multiplied by the number of days of nonpayment, up to 30, whether the employee is part-time or full-time and whether he is paid on an hourly or salaried basis.  (Mamika v. Barca (1998) 68 Cal.App.4th 487.)  When an employee is discharged, the final wages are due within 24 hours of the discharge.   
-At this early stage, we estimate a 50% chance of prevailing based on Plaintiff missed rest period claims.  
-7.	Failure To Reimburse 
-Gonzalez claims DSE violated California Labor Code Section 2802 by failing to reimburse him for its business expenses for purchasing tools for the job. “The elements of a [section 2802(a)] cause of action, as delineated by the statutory language, are: (1) the employee made expenditures or incurred losses; (2) the expenditures or losses were incurred in direct consequence of the employee’s discharge of his or her duties, or obedience to the directions of the employer; and (3) the expenditures or losses were necessary.”(Gallano v. Burlington Coat Factory of California, LLC (2021) 67 Cal.App.5th 953, 960.)
-Gonzalez was given a debit card to make all such purchases during his employment up until June 30, 2023. Thus, the only time he could have been forced to do so was from July 1, 2023, through his termination on September 8, 2023. We have not seen any evidence support his claims that he was not compensated for any purchases he now complains of. 
-Thus, at this time, we are not aware of any facts that would give rise to liability for this cause of action.   
-Damages Analysis
-If successful on his whistleblower retaliation claims, Gonzalez may be entitled to back pay, front pay, compensatory damages for emotional distress, special damages for medical treatment, punitive damages, and attorneys’ fees. For the wage and hour claims, there are damages for unpaid wages along with penalties.
-1.	Backpay
-Gonzalez can recover backpay if he prevails on his causes of action based on retaliation based on 
-the Labor Code and constructive discharge in violation of public policy. Back pay is the compensation, including benefits, in the amount the employee would have received, but for the adverse employment action, less sums obtained through mitigation. (Parker v. Twentieth Century- Fox Film Corp. (1970) 3 Cal.3d 176, 181.) Back pay awards are measured from the time of the adverse action until the date of judgment. Although not an automatic or mandatory remedy, there is a strong presumption in favor of back pay awards to victims of retaliation. 
-Gonzalez has failed to produce records showing his efforts to obtain subsequent employment since his layoff from DSE, but we will follow up with his attorney to obtain them.  Assuming Reyes can meet his burden to mitigate his damages and trial is set one year out (4/30/25), then Gonzalez’s back pay claim at trial would be $75,384 = (349 workdays x [$27 x 8]) minus the amounts he has earned in mitigation. More than likely, his mitigation income would be at least 75% of his DSE earnings, which would reduce his claimed backpay damages to $18,846. We also note that Plaintiff could claim front pay (from the date of the trial into the future), but such awards are more common when a plaintiff is elderly and not likely to find replacement employment, or where the plaintiff had extremely long-term employment with the defendant. For our purposes, we do not presently assess a likelihood of a front pay award.
-2.	Emotional Distress Damages
-Gonzalez can recover emotional distress damages for his causes of action based on retaliation based on the Labor Code, and wrongful termination in violation of public policy. 
-At this pre-deposition stage, it is difficult to estimate the potential emotional distress damages Gonzalez may seek. He provided no documents to suggest treatment for his emotional distress damages. Should this case not resolve pre-litigation, at Gonzalez’s deposition, and through further written discovery, we will explore any mental or physical health treatments he may have received, any medications he may be taking, how any alleged emotional distress affects his daily life activities, alternative stressors, and increasing severity of any emotional distress he alleges since his termination. We will also assess his credibility as a witness and the extent of his emotional distress since his last date of employment with DSE. While there are cases with egregious facts where employees have been awarded millions of dollars in emotional distress damages, this case does not appear to fall within that category. The typical emotional distress damages awarded in employment law cases is approximately $150,000 to $600,000, with these potential damages being valued less at mediation.
-Given that we do not assess a strong likelihood of prevailing on those claims and that the documents show Plaintiff resigned for other work opportunities and therefore did not suffer the typical distress a terminated employee might suffer, we assess his claims to be garden variety or roughly between $25,000 - $50,000.
-3.	Meal Break Penalties
-As discussed above, there is no clear documentation of whether Gonzalez received a meal break before or at each fifth hour worked. If DSE is unable to establish that Gonzalez had the opportunity to have a thirty-minute uninterrupted meal break prior to the fifth hour, then he would be owed one hour’s pay for each of these occurrences. From September 11, 2021, through March 18, 2022 (117 workdays), assuming DSE failed to provide Gonzalez a meal break on each day worked, Gonzalez would be owed $2,691  (177 x $23). From March 19, 2022, through September 8, 2023 (366 workdays), assuming DSE failed to provide Gonzalez a meal break on each day worked, Gonzalez would be owed $9,882  (366 x $27). Thus, the maximum exposure from this claim is $12,573. 
-4.	Rest Break Penalties 
-As discussed above, there is no documentation of whether Gonzalez received a rest break before or at each fourth hour worked. If DSE is unable to establish that Gonzalez had the opportunity to have a ten-minute uninterrupted rest break prior to each fourth hour worked, then he would be owed one hour’s pay for each of these occurrences, as follows:  
-From September 11, 2021, through March 18, 2022 (117 workdays), assuming DSE failed to provide Gonzalez a rest break on each day worked, Gonzalez would be owed $2,691  (177 x $23). From March 19, 2022, through September 8, 2023 (366 workdays), assuming DSE failed to provide Gonzalez a rest break on each day worked, Gonzalez would be owed $9,882  (366 x $27). Thus, the maximum exposure from this claim is $12,573. 
-5.	Labor Code § 1102.5 Penalty
-An employee who prevails on a Labor Code § 1102.5 claim may get remedies including a civil penalty of up to $10,000, per violation. Thus, if Plaintiffs prevail on their retaliation claims they could be awarded $10,000 each. 
-6.	Waiting Time Penalty
-The maximum penalty allowable for this claim is 30 days’ pay or $6,480. 
-7.	Attorneys’ Fees and Costs
-Under the Labor Code, a prevailing plaintiff is entitled to their attorneys’ fees. Gonzalez’s counsel is likely working under a contingency fee arrangement. However, at the conclusion of the litigation, if he prevailed, Gonzalez would petition for a fee award, which considers all of the hours their attorney worked, multiplied by a fabricated hourly rate. These attorneys’ fees awards are mandatory for a prevailing Gonzalez. If this case proceeds through trial, we estimate Gonzalez’s award of attorneys’ fees will be in the range of $550,000 to $750,000.  To date, we estimate that Plaintiffs’ counsel has incurred approximately $5,000 in fees and costs preparing his personnel records demand, settlement demand, and related settlement communications. 
-8.	Punitive Damages
-Punitive damages are available if a plaintiff can establish by clear and convincing evidence, that the employer is guilty of oppression, fraud, or malice, and acted with an intent to vex, injure, or annoy, or with a conscious disregard of her rights.  Cal. Civ. Code section 3294, subd.(a).  Based on the facts known to date, we do not assess a likelihood of punitive damages for Gonzalez.
-Settlement Value And Recommendation
-Using this calculation, we analyze potential settlement value based on traditional valuation metrics: each category of potential damages multiplied by the likelihood of Plaintiffs’ success at trial + attorneys’ fees and costs to date. Based on the traditional valuation metrics, we currently estimate the settlement valuation of the case at time of trial to be approximately $148,463 – $349,713, calculated as follows:   
-Gonzalez’s Backpay Through Trial:                        $18,846 x 45% = $8,481
-Emotional Distress Damages:                                  ($25,000-$50,000) x 45% =
-$11,250 - $22,500
-Meal Break Penalties:                                                 $12,573 x 40% = $5,658
-Rest Break Penalties:                                                  $12,573 x 40% = $5,658
-Labor Code § 1102.5 Penalty:                                  $10,000 x 45% = $4,500
-Waiting Time Penalty:                                                  $6,480 x 45% = $2,916
-Attorneys’ Fees:                                                              $550,000 – $750,000 x 20 – 40% = 
-$110,000 - $300,000   
-Punitive Damages:                                                        $0  
-Total Settlement Value At Trial:                                               $148,463 – $349,713
-Since DSE made its opening settlement offer of $5,000, Gonzalez has made a reduced settlement demand of $85,000 to resolve his claims in this matter. Our recommendation is to continue settlement discussions that were already ongoing between Gonzalez and DSE to potentially resolve this matter early before further litigation runs up the lion’s share of Gonzalez’s damages – their attorneys’ fees and costs. Based on our current estimate of Gonzalez’s attorneys' fees and costs ($5,000), our current assessment of the value of his case is between $43,463 - $54,713. 
-A prerequisite to continuing informal settlement discussions, we will demand Gonzalez produce documents in support of his emotional distress claims, and search for and earnings from any subsequent employment.  We will provide an updated assessment after this information is obtained. Should you have any questions or concerns, please contact us. 
-Warmly,”
-Imran Rahman
-Associate Attorney
-1 Embarcadero Center| Suite 2100| San Francisco | CA | 94111
-8050 N. Palm. Ave | Suite 300 | Fresno | CA | 93711
-DIR 415-275-3548
- &lt;https://ohaganmeyer.com/&gt; 
-From: Cruz Zavala &lt;czavala@ohaganmeyer.com &lt;mailto:czavala@ohaganmeyer.com&gt; &gt; 
-Sent: Tuesday, July 2, 2024 11:04 AM
-To: Imran Rahman &lt;irahman@ohaganmeyer.com &lt;mailto:irahman@ohaganmeyer.com&gt; &gt;
-Subject: RE: Ramiro Gonzalez v. DS Electric, Inc. - Berkley Claim No.: 49538 [EXTERNAL] [IMAN-ACTIVE.FID448525]
-Tomorrow works. I am in mediation today. 
-Cruz Zavala
-Associate Attorney
-One Embarcadero Center | Suite 2100 | San Francisco | CA | 94111 
-PH 312.422.6100 | DIR 415.275.3546
-From: Imran Rahman &lt;irahman@ohaganmeyer.com &lt;mailto:irahman@ohaganmeyer.com&gt; &gt; 
-Sent: Tuesday, July 2, 2024 10:15 AM
-To: Cruz Zavala &lt;czavala@ohaganmeyer.com &lt;mailto:czavala@ohaganmeyer.com&gt; &gt;
-Subject: RE: Ramiro Gonzalez v. DS Electric, Inc. - Berkley Claim No.: 49538 [EXTERNAL] [IMAN-ACTIVE.FID448525]
-Hi Cruz, 
-Didn’t get to this yesterday. Do you have availability today or tomorrow around noon?  
-Imran Rahman
-Associate Attorney
-1 Embarcadero Center| Suite 2100| San Francisco | CA | 94111
-8050 N. Palm. Ave | Suite 300 | Fresno | CA | 93711
-DIR 415-275-3548
- &lt;https://ohaganmeyer.com/&gt; 
-From: Cruz Zavala &lt;czavala@ohaganmeyer.com &lt;mailto:czavala@ohaganmeyer.com&gt; &gt; 
-Sent: Friday, June 28, 2024 4:27 PM
-To: Imran Rahman irahman@ohaganmeyer.com &lt;mailto:irahman@ohaganmeyer.com&gt; 
-Subject: RE: Ramiro Gonzalez v. DS Electric, Inc. - Berkley Claim No.: 49538 [EXTERNAL] [IMAN-ACTIVE.FID448525]
-1230 okay? 
-Cruz Zavala
-Associate Attorney
-One Embarcadero Center | Suite 2100 | San Francisco | CA | 94111 
-PH 312.422.6100 | DIR 415.275.3546
-From: Imran Rahman &lt;irahman@ohaganmeyer.com &lt;mailto:irahman@ohaganmeyer.com&gt; &gt; 
-Sent: Friday, June 28, 2024 4:10 PM
-To: Cruz Zavala &lt;czavala@ohaganmeyer.com &lt;mailto:czavala@ohaganmeyer.com&gt; &gt;
-Subject: FW: Ramiro Gonzalez v. DS Electric, Inc. - Berkley Claim No.: 49538 [EXTERNAL] [IMAN-ACTIVE.FID448525]
-Hey Cruz, 
-I got a hold of the guy. Turns out his English is not so bad. Spanish translation I think would be helpful but not necessary. Do you have time Monday at noon to call him together? If not, no worries. 
-Thanks! 
-Imran Rahman
-Associate Attorney
-1 Embarcadero Center| Suite 2100| San Francisco | CA | 94111
-8050 N. Palm. Ave | Suite 300 | Fresno | CA | 93711
-DIR 415-275-3548
- &lt;https://ohaganmeyer.com/&gt; 
-From: Imran Rahman 
-Sent: Monday, June 24, 2024 3:59 PM
-To: Daniel Suarez &lt;dselectric3@gmail.com &lt;mailto:dselectric3@gmail.com&gt; &gt;
-Cc: Daniel Cravens &lt;dcravens@ohaganmeyer.com &lt;mailto:dcravens@ohaganmeyer.com&gt; &gt;; Levinsky, Heather &lt;hlevinsky@berkleyselect.com &lt;mailto:hlevinsky@berkleyselect.com&gt; &gt;; Cruz Zavala &lt;czavala@ohaganmeyer.com &lt;mailto:czavala@ohaganmeyer.com&gt; &gt;
-Subject: RE: Ramiro Gonzalez v. DS Electric, Inc. - Berk</t>
-        </is>
-      </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>RE: Ramiro Gonzalez v. DS Electric, Inc. - Berkley Claim No.: 49538 [EXTERNAL] [IMAN-ACTIVE.FID448525]</t>
-        </is>
-      </c>
-      <c r="V2" t="inlineStr">
-        <is>
-          <t>Gonzalez v. DS Electric, Inc.</t>
+          <t>Email communication with Imran Rahman regarding Ramiro Gonzalez v. DS Electric, Inc. - Berkley Claim No.: 49538.</t>
         </is>
       </c>
     </row>
@@ -800,15 +607,11 @@
           <t>DCRA</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>1014</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>35348</t>
-        </is>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -843,39 +646,6 @@
           <t>Email communication with IT Support concerning sending large attachments outside the firm.</t>
         </is>
       </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">The firm uses ShareFile to securely send media to external parties. It is essentially a more secure DropBox.
-It looks like you already have a license assigned to you, let me know if you have any questions or concerns.
-Thanks, 
-Ryan J. Smith
-IT Support Tech 
-One E Wacker Dr.  | Suite 3400  | Chicago |  IL  | 60601
-PH 312.422.6100 |  DIR 312.422.6112 |  FX 312.422.6110 
-From: Daniel Cravens &lt;dcravens@ohaganmeyer.com&gt; 
-Sent: Thursday, July 25, 2024 2:26 PM
-To: IT Support &lt;ITSupport@ohaganmeyer.com&gt;
-Subject: Sending large attachments
-Hi,
-What is the process for email large attachments outside the firm?
-Daniel J. Cravens
-Fresno Managing Partner
-8050 N. Palm Ave. | Suite 300 | Fresno | CA | 93711
-DIR 415.604.0142 | CEL 559.472.6584
- &lt;https://ohaganmeyer.com/&gt; 
-</t>
-        </is>
-      </c>
-      <c r="U3" t="inlineStr">
-        <is>
-          <t>RE: Sending large attachments</t>
-        </is>
-      </c>
-      <c r="V3" t="inlineStr">
-        <is>
-          <t>Based on the information provided in the email, the inferred client alias is None.</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -896,15 +666,11 @@
           <t>DCRA</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>1014</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>35348</t>
-        </is>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -936,55 +702,7 @@
       <c r="R4" t="inlineStr"/>
       <c r="S4" t="inlineStr">
         <is>
-          <t>Email communication with Ms. Yu concerning meet and confer for Wang et al. v. Harris et al. (Case No. CIVSB2412923) to avoid demurrer and discuss potential resolution.</t>
-        </is>
-      </c>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Received, thank you. Once you send it back with your edits, I will get it out the door. 
-Nicole Tavis
-One Embarcadero Center | Suite 2100 | San Francisco | CA | 94111
-PH 415-578-6900 | DIR 415.604.0209 
-From: Daniel Cravens &lt;dcravens@ohaganmeyer.com&gt; 
-Sent: Thursday, July 25, 2024 3:09 PM
-To: Nicole Tavis &lt;ntavis@ohaganmeyer.com&gt;
-Subject: FW: Wang et al. v. Harris et al. (Case No. CIVSB2412923)
-Email for the 431.30 declaration, Exhibit B.
-Daniel J. Cravens
-Fresno Managing Partner
-8050 N. Palm Ave. | Suite 300 | Fresno | CA | 93711
-DIR 415.604.0142 | CEL 559.472.6584
-From: Daniel Cravens 
-Sent: Thursday, July 25, 2024 3:08 PM
-To: lawyerym@hotmail.com &lt;mailto:lawyerym@hotmail.com&gt; 
-Subject: Wang et al. v. Harris et al. (Case No. CIVSB2412923)
-Dear Ms. Yu,
-I am writing to meet and confer as required by CCP section 431.30 concerning the second and third cases of action alleged against Sanchez, Ortiz, and Real in the hope of avoiding a demurrer.
-These causes of action depend on a fiduciary relationship between Real and its agents on the one hand and Plaintiff on the other.  However, the complaint discloses that no such relationship existed.
-*	Paragraph 16 avers that Harris filed a Partition Complaint against your client for division of the property and obtained a default judgment against your client.
-*	Paragraph 18 avers that the Court appointed an elisor to act on behalf of your client.
-*	Paragraph 19 avers that the Plaintiff applied for relief ex parte which the Court denied.
-The allegation that the property was sold pursuant to a court partition order and after the appointment of an elisor establishes that there can be no breach of fiduciary relationship or breach of duty of care by Real and its agents.
-Moreover, the allegation that your client reposed “repos[ed] trust and confidence in Defendants in connection with listing of the Property (¶ 46) is directly contradicted by the allegation that your client was “unaware of the Property’s sale until March 8th, 2024.”  The allegation that your client reposed trust in Real and its agents is false and brought in bad faith.
-We would like to avoid unnecessary expenditure of fees bringing a demurrer and 128.7 motion. Do you have time to discuss this matter next week? I have broad availability on July 30 and July 31.
-Regards,
-Dan 
-Daniel J. Cravens
-Fresno Managing Partner
-8050 N. Palm Ave. | Suite 300 | Fresno | CA | 93711
-DIR 415.604.0142 | CEL 559.472.6584
- &lt;https://ohaganmeyer.com/&gt; 
-</t>
-        </is>
-      </c>
-      <c r="U4" t="inlineStr">
-        <is>
-          <t>RE: Wang et al. v. Harris et al. (Case No. CIVSB2412923)</t>
-        </is>
-      </c>
-      <c r="V4" t="inlineStr">
-        <is>
-          <t>None</t>
+          <t>Email communication with Ms. Yu concerning meeting and conferring on the second and third causes of action in Wang et al. v. Harris et al. (Case No. CIVSB2412923) to avoid a demurrer.</t>
         </is>
       </c>
     </row>

</xml_diff>